<commit_message>
fixes and other other other
</commit_message>
<xml_diff>
--- a/ozon_products.xlsx
+++ b/ozon_products.xlsx
@@ -434,17 +434,17 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="12" customWidth="1" min="1" max="1"/>
-    <col width="181" customWidth="1" min="2" max="2"/>
-    <col width="8" customWidth="1" min="3" max="3"/>
+    <col width="198" customWidth="1" min="2" max="2"/>
+    <col width="11" customWidth="1" min="3" max="3"/>
     <col width="21" customWidth="1" min="4" max="4"/>
     <col width="17" customWidth="1" min="5" max="5"/>
     <col width="7" customWidth="1" min="6" max="6"/>
     <col width="9" customWidth="1" min="7" max="7"/>
     <col width="15" customWidth="1" min="8" max="8"/>
-    <col width="22" customWidth="1" min="9" max="9"/>
+    <col width="24" customWidth="1" min="9" max="9"/>
     <col width="37" customWidth="1" min="10" max="10"/>
-    <col width="124" customWidth="1" min="11" max="11"/>
-    <col width="189" customWidth="1" min="12" max="12"/>
+    <col width="156" customWidth="1" min="11" max="11"/>
+    <col width="181" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -512,32 +512,32 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1393129475</t>
+          <t>2003611123</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Кран шаровой 3" вн-вн (2 шт) VALTEC BASE со стальной рукояткой, полнопроходной / Латунная запорная арматура ДУ 80 с рычагом для системы отопления и водоснабжения, арт. VT.214.N.11</t>
+          <t>Poco Смартфон C75 EU 6/128 ГБ, черный</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Valtec</t>
+          <t>Poco</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>38304</t>
+          <t>8947</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>40751</t>
+          <t>9406</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>83950</t>
+          <t>39999</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -547,175 +547,175 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>1 отзыв</t>
+          <t>1 310 отзывов</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>TradeON</t>
+          <t>SV SMARTPHONE</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>https://www.ozon.ru/seller/1647152/</t>
+          <t>https://www.ozon.ru/seller/1685463/</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>ИП Адамович Виктор Иосифович; 324774600001498</t>
+          <t>ИП Соболь Влада Владимировна; 324290000003171</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>https://www.ozon.ru/product/kran-sharovoy-3-vn-vn-2-sht-valtec-base-so-stalnoy-rukoyatkoy-polnoprohodnoy-latunnaya-1393129475/?at=LZtlDKWjxIjlZKGTR62l7NF2y971yCyMPX7LuXERWgB</t>
+          <t>https://www.ozon.ru/product/poco-smartfon-c75-eu-6-128-gb-chernyy-2003611123/?at=gpt41jwomszPg4nQs589RxOsWQvnKEhDgkjBKcGB1DVz</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1968173288</t>
+          <t>2006925323</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>комплект угловых кранов 1/2 для подключения гибкой подводки смесителя или водонагревателя (2 шт.)</t>
+          <t>Tecno Смартфон CAMON 40 Ростест (EAC) 8/256 ГБ, черный</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Краны</t>
+          <t>Tecno</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>590</t>
+          <t>18314</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>632</t>
+          <t>18880</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2800</t>
+          <t>23990</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>4.5</t>
+          <t>4.9</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2 отзыва</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Душевое Удовольствие</t>
-        </is>
-      </c>
+          <t>208 отзывов</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr">
         <is>
-          <t>https://www.ozon.ru/seller/2426385/</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>ООО ООО "ЮАНЬ ЧЖЭН ЭЛЕКТРОННАЯ КОММЕРЦИЯ"143444, Россия, Московская Область, Красногорск, Геологов, 2, 4,; 221245000067311</t>
-        </is>
-      </c>
+          <t>https://www.ozon.ru/seller/236588/</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr">
         <is>
-          <t>https://www.ozon.ru/product/komplekt-uglovyh-kranov-1-2-dlya-podklyucheniya-gibkoy-podvodki-smesitelya-ili-vodonagrevatelya-1968173288/?at=WPtNLOE97FoKj0QGsJB8x0PCVzqvz9TZOMAEnf9knEKZ</t>
+          <t>https://www.ozon.ru/product/tecno-smartfon-camon-40-rostest-eac-8-256-gb-chernyy-2006925323/?at=MZtvyLkwRfqOVN7jcgWw3BjtVXJ9vzCqDmJKPs2BwDvY</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2157665596</t>
+          <t>2133543492</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Шаровый кран Bugatti Oregon 322 с американкой 1/2", бабочка, ВР-НР, комплект</t>
+          <t>iQOO Смартфон Z10 Ростест (EAC) 8/256 ГБ, черный</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Краны</t>
+          <t>iQOO</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>766</t>
+          <t>20106</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>821</t>
+          <t>21219</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>1580</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
+          <t>35999</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>10 отзывов</t>
+        </is>
+      </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>СантехЛидер</t>
+          <t>iQOO Official Store</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>https://www.ozon.ru/seller/1468932/</t>
+          <t>https://www.ozon.ru/seller/2898162/</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>ИП Смирнова Светлана Николаевна; 309504325900023</t>
+          <t>ООО ООО "БАЙТ БУМ"127287, Россия, Москва, г Москва, ул Хуторская 2-я, стр 23, д 38А,; 131257700003538</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>https://www.ozon.ru/product/sharovyy-kran-bugatti-oregon-322-s-amerikankoy-1-2-babochka-vr-nr-komplekt-2157665596/?at=z6tOY61glc7x9G3YCMGzEVOiyZBj9KSv6pVkriMGmKl5</t>
+          <t>https://www.ozon.ru/product/iqoo-smartfon-z10-rostest-eac-8-256-gb-chernyy-2133543492/?at=08tYX9g7McP6qr4QSEpQ9REc7kR46DsLwr80VIA2ownp</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1319117444</t>
+          <t>1771387609</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Кран шаровый 1/2" с внутренней и наружной резьбой (2 шт), ГАЛЛОП, серия "Практик"</t>
+          <t>realme Смартфон Note 60X Ростест (EAC) 3/64 ГБ, черный</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Галлоп</t>
+          <t>realme</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>688</t>
+          <t>4273</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>735</t>
+          <t>4999</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>1600</t>
+          <t>8499</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -725,237 +725,245 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>2 868 отзывов</t>
+          <t>7 034 отзыва</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>AZEL</t>
+          <t>realme</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>https://www.ozon.ru/seller/1373437/</t>
+          <t>https://www.ozon.ru/seller/216243/</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>ИП Фатхуллина Эльвира Гумяровна, ИП; 323730000050351</t>
+          <t>ООО ООО "РМ КОММЬЮНИКЕЙШН"115280, г. Москва, вн.тер.г. Муниципальный округ Даниловский, улица Ленинская Слобода, Д. 19, помещение 21В/1H/5.1; 197746267355</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>https://www.ozon.ru/product/kran-sharovyy-1-2-s-vnutrenney-i-naruzhnoy-rezboy-2-sht-gallop-seriya-praktik-1319117444/?at=lRt6wxrnJTGZ19w3fp9EYR9cyQZ15xszMr4M4IQqlP74</t>
+          <t>https://www.ozon.ru/product/realme-smartfon-note-60x-rostest-eac-3-64-gb-chernyy-1771387609/?at=mqtko7PgAcEl1Y10coOx5McRM6BQJUojZmZ0UK6GZWY</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1359745044</t>
+          <t>1869776225</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Кран шаровый 1/2" ВРхВР Veher, 1 шт латунь, ручка рычаг / кран шаровый ДУ15 латунный</t>
+          <t>Redmi Смартфон 8/256 ГБ, черный</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>VEHER</t>
+          <t>Redmi</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>276</t>
+          <t>5901</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>296</t>
+          <t>6217</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>743</t>
+          <t>13999</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>4.8</t>
+          <t>4.4</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>2 088 отзывов</t>
+          <t>466 отзывов</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>РУСХИТ</t>
+          <t>Bao Phone</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>https://www.ozon.ru/seller/1369103/</t>
+          <t>https://www.ozon.ru/seller/2597173/</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>ООО "Р-СЕРВИС"129226, г. Москва, ул. Сельскохозяйственная, д.11, корп.3, эт.1, пом.II, ком.1 (РМ140)1; 227700433850</t>
+          <t>ИП Идалов Ибрагим Усманович; 321200000013285</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>https://www.ozon.ru/product/kran-sharovyy-1-2-vrhvr-veher-1-sht-latun-ruchka-rychag-kran-sharovyy-du15-latunnyy-1359745044/?at=x6tP5klM6hYzgnR2uDzgQMjsq84KRlIBXvBwlCxl3559</t>
+          <t>https://www.ozon.ru/product/redmi-smartfon-8-256-gb-chernyy-1869776225/?at=DqtDLWJEnuj1wKBks45Lo6otB73YGlhPY3ZnoSlmOxMm</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2175895852</t>
+          <t>1711714454</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Кран шаровой 1/2" для воды со встроенным фильтром и редуктором давления, универсальный Valtec, VT.300</t>
+          <t>Tecno Смартфон Spark 30 5G Ростест (EAC) 6/128 ГБ, черный</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Valtec</t>
+          <t>Tecno</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>3055</t>
+          <t>10011</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>3259</t>
+          <t>10524</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>4938</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
+          <t>19990</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>4.9</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>971 отзыв</t>
+        </is>
+      </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Акваинженер</t>
+          <t>TECNO STORE</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>https://www.ozon.ru/seller/1344879/</t>
+          <t>https://www.ozon.ru/seller/1452131/</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>ООО ООО "АКВАИНЖЕНЕР"308008, г Белгород, ул Восточная, , д 71, 71; 233100010164</t>
+          <t>ООО ООО "КИБЕР ЭНЕРДЖИ"127238, Россия, Москва, г Москва, Дмитровское шоссе, к 2, д; 321237700690864</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>https://www.ozon.ru/product/kran-sharovoy-1-2-dlya-vody-so-vstroennym-filtrom-i-reduktorom-davleniya-universalnyy-valtec-vt-300-2175895852/?at=x6tP5klM6hmLqDARsyoO5RPTW3x2N5tVjEORyhm37yBV</t>
+          <t>https://www.ozon.ru/product/tecno-smartfon-spark-30-5g-rostest-eac-6-128-gb-chernyy-1711714454/?at=vQtrnPLY2tPD6WAphBNjgR5uQzJvkOu1oy4DZHpYNjy6</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>368154455</t>
+          <t>1897984574</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Кран шаровой латунный 3/4" дюйма KOER (Чехия) DN20 вн/вн ручка рычаг</t>
+          <t>Смартфон 6,5-дюймовый противоударный смартфон Note60x, смартфон на базе Android 13, смартфон с большим объемом памяти, смартфон для студентов, поддержка русского языка Global 8/256 ГБ, черно-серый</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>KOER</t>
+          <t>Смартфоны</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>681</t>
+          <t>3037</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>728</t>
+          <t>3233</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>1922</t>
+          <t>3773</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>4.9</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>48 отзывов</t>
+          <t>216 отзывов</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Сантехника161.рф</t>
+          <t>Флагманский магазин UP</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>https://www.ozon.ru/seller/240825/</t>
+          <t>https://www.ozon.ru/seller/2489768/</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>ИП Филин Артур Александрович; 319619600234071</t>
+          <t>Yaofengbaihuo</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>https://www.ozon.ru/product/kran-sharovoy-latunnyy-3-4-dyuyma-koer-chehiya-dn20-vn-vn-ruchka-rychag-368154455/?at=83tB51GvVIV1R766tLkql10clkJwELfY35vqPsZypOV4</t>
+          <t>https://www.ozon.ru/product/smartfon-6-5-dyuymovyy-protivoudarnyy-smartfon-note60x-smartfon-na-baze-android-13-smartfon-1897984574/?at=GRt2NPOD0ck9ZDXzuNYNgNgHqy77nqiORKk4GIm79JBr</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2081631649</t>
+          <t>1743461395</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Кран шаровый полипропиленовый PPR D20 (10 шт.) для холодной и горячей воды, отопления</t>
+          <t>Tecno Смартфон Spark 30 Ростест (EAC) 8/256 ГБ, черный</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Краны</t>
+          <t>Tecno</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>647</t>
+          <t>10633</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>692</t>
+          <t>11179</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>1599</t>
+          <t>18990</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -965,59 +973,59 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>92 отзыва</t>
+          <t>3 053 отзыва</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>AV-GROUP</t>
+          <t>TECNO STORE</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>https://www.ozon.ru/seller/2885313/</t>
+          <t>https://www.ozon.ru/seller/1452131/</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>ИП Белоус Евгений Анатольевич; 325665800094191</t>
+          <t>ООО ООО "КИБЕР ЭНЕРДЖИ"127238, Россия, Москва, г Москва, Дмитровское шоссе, к 2, д; 321237700690864</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>https://www.ozon.ru/product/kran-sharovyy-polipropilenovyy-ppr-d20-10-sht-dlya-holodnoy-i-goryachey-vody-otopleniya-2081631649/?at=k2toy9EWVTx87DEETQ12lVZcYpnmv4cr3p8lMiMn66Kk</t>
+          <t>https://www.ozon.ru/product/tecno-smartfon-spark-30-rostest-eac-8-256-gb-chernyy-1743461395/?at=28t024ZBRf1L62mrCrRoX7nUl183plT4l4g3yfzPQ6rP</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>1410819107</t>
+          <t>2137918430</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Шаровой кран ROMMER RBV-0002-2210320 3/4" ВН/НР ручка рычаг</t>
+          <t>iQOO Смартфон Neo 10 Ростест (EAC) 16/512 ГБ, черный, черно-серый</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>ROMMER</t>
+          <t>iQOO</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>406</t>
+          <t>37482</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>423</t>
+          <t>39635</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>532</t>
+          <t>52999</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -1027,59 +1035,59 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>261 отзыв</t>
+          <t>11 отзывов</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Jakko</t>
+          <t>iQOO Official Store</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>https://www.ozon.ru/seller/1384222/</t>
+          <t>https://www.ozon.ru/seller/2898162/</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>ООО ООО "ТЕХСТРОЙТОРГ"142032, Россия, Московская Область, г Домодедово, Сиреневая аллея, 1, д 1А, 3 ком. 11; 235000056422</t>
+          <t>ООО ООО "БАЙТ БУМ"127287, Россия, Москва, г Москва, ул Хуторская 2-я, стр 23, д 38А,; 131257700003538</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>https://www.ozon.ru/product/sharovoy-kran-rommer-rbv-0002-2210320-3-4-vn-nr-ruchka-rychag-1410819107/?at=28t021YlqTLnDEDBfG3rQ8ZUlpGg6NfENMY07HAKXz4B</t>
+          <t>https://www.ozon.ru/product/iqoo-smartfon-neo-10-rostest-eac-16-512-gb-chernyy-cherno-seryy-2137918430/?at=DqtDLWJEnu2BPmlPhOOk5kqckvYk78h9NmxwVckyxK85</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>368096794</t>
+          <t>1469526277</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Кран шаровой латунный 1/2" дюйма KOER (Чехия) DN15 вн/нар ручка бабочка</t>
+          <t>Tecno Смартфон POVA 6 Pro 5G Ростест (EAC) 12/256 ГБ, черный</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>KOER</t>
+          <t>Tecno</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>575</t>
+          <t>22806</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>616</t>
+          <t>24069</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2200</t>
+          <t>38337</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -1089,27 +1097,27 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>72 отзыва</t>
+          <t>2 221 отзыв</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Сантехника161.рф</t>
+          <t>TECNO STORE</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>https://www.ozon.ru/seller/240825/</t>
+          <t>https://www.ozon.ru/seller/1452131/</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>ИП Филин Артур Александрович; 319619600234071</t>
+          <t>ООО ООО "КИБЕР ЭНЕРДЖИ"127238, Россия, Москва, г Москва, Дмитровское шоссе, к 2, д; 321237700690864</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>https://www.ozon.ru/product/kran-sharovoy-latunnyy-1-2-dyuyma-koer-chehiya-dn15-vn-nar-ruchka-babochka-368096794/?at=79tnXlgp5sN0V0Vmc9Q717h76ngYXtApGrpAf80jBly</t>
+          <t>https://www.ozon.ru/product/tecno-smartfon-pova-6-pro-5g-rostest-eac-12-256-gb-chernyy-1469526277/?at=Y7tjWvpnNClrrYVXuXvOzD3hYX1vywtNlAkYKTQo0Zql</t>
         </is>
       </c>
     </row>

</xml_diff>